<commit_message>
Accreditamento ArchiMed: aggiornamento report-checklist.xlsx
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#090903000000XX/AOUCAREGGI/ARCHIMED/8.48/report-checklist.xlsx
+++ b/GATEWAY/A1#090903000000XX/AOUCAREGGI/ARCHIMED/8.48/report-checklist.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="284">
   <si>
     <t xml:space="preserve">COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -422,7 +422,7 @@
     <t xml:space="preserve">NO</t>
   </si>
   <si>
-    <t xml:space="preserve">In caso di errore verrà coinvolto l’ufficio idoneo alla sua correzione</t>
+    <t xml:space="preserve">L'invio al gateway è asincrono e il medico prosegue con la propria attività. In caso di errore viene inviata al medico e al personale amministrativo una notifica. Dopo che l'errore è stato corretto dal medico o dal personale amministrativo, il referto può essere firmato nuovamente e inviato alla coda che in maniera automatica e schedulata (intervallo configurabile) ritenta l’invio verso il gateway </t>
   </si>
   <si>
     <t xml:space="preserve">KO</t>
@@ -494,7 +494,7 @@
 Per questo caso di test è richiesta la  sola descrizione del comportamento a fronte di un timeout, da inserire nella colonna "J" nominata come "GESTIONE ERRORE".</t>
   </si>
   <si>
-    <t xml:space="preserve">Il documento viene inserito nella coda per un ulteriore tentativo di validazione</t>
+    <t xml:space="preserve">In caso di timeout con il gateway il processo clinico prosegue, il referto viene prodotto. Il documento viene aggiunto alla coda che in maniera automatica e schedulata (intervallo configurabile) ritenta l’invio verso il gateway</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT5_KO</t>
@@ -509,6 +509,9 @@
   </si>
   <si>
     <t xml:space="preserve">2.16.840.1.113883.2.9.2.90903.45c9c160458635a842a60b21f2db53b82a1a6d5d071ffca01fa8fc826915cbf3.2fc5e5addb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'invio al gateway è asincrono e il medico prosegue con la propria attività. In caso di errore viene inviata al medico e al personale amministrativo una notifica. Dopo che l'errore è stato corretto dal medico, il referto può essere firmato nuovamente e inviato alla coda che in maniera automatica e schedulata (intervallo configurabile) ritenta l’invio verso il gateway </t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT6_KO</t>
@@ -1864,11 +1867,11 @@
   <dimension ref="A1:T581"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="J25" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
-      <selection pane="bottomRight" activeCell="I55" activeCellId="0" sqref="I55"/>
+      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="bottomRight" activeCell="P53" activeCellId="0" sqref="P53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2282,7 +2285,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="114.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="25" t="n">
         <v>29</v>
       </c>
@@ -2334,7 +2337,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="25" t="n">
         <v>37</v>
       </c>
@@ -2386,7 +2389,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="25" t="n">
         <v>45</v>
       </c>
@@ -2420,7 +2423,7 @@
       <c r="S16" s="31"/>
       <c r="T16" s="32"/>
     </row>
-    <row r="17" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="25" t="n">
         <v>63</v>
       </c>
@@ -2463,7 +2466,7 @@
         <v>56</v>
       </c>
       <c r="P17" s="29" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="Q17" s="29"/>
       <c r="R17" s="30"/>
@@ -2472,7 +2475,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="25" t="n">
         <v>64</v>
       </c>
@@ -2483,22 +2486,22 @@
         <v>49</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E18" s="27" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F18" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G18" s="28" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H18" s="28" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I18" s="28" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J18" s="29" t="s">
         <v>56</v>
@@ -2524,7 +2527,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="25" t="n">
         <v>65</v>
       </c>
@@ -2535,22 +2538,22 @@
         <v>49</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F19" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G19" s="28" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H19" s="28" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I19" s="28" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J19" s="29" t="s">
         <v>56</v>
@@ -2567,7 +2570,7 @@
         <v>56</v>
       </c>
       <c r="P19" s="29" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="Q19" s="29"/>
       <c r="R19" s="30"/>
@@ -2576,7 +2579,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="25" t="n">
         <v>66</v>
       </c>
@@ -2587,22 +2590,22 @@
         <v>49</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F20" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G20" s="28" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H20" s="28" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I20" s="28" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J20" s="29" t="s">
         <v>56</v>
@@ -2628,7 +2631,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="25" t="n">
         <v>67</v>
       </c>
@@ -2639,22 +2642,22 @@
         <v>49</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F21" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G21" s="28" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H21" s="28" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I21" s="28" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J21" s="29" t="s">
         <v>56</v>
@@ -2680,7 +2683,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="25" t="n">
         <v>68</v>
       </c>
@@ -2691,22 +2694,22 @@
         <v>49</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F22" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G22" s="28" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H22" s="28" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I22" s="28" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J22" s="29" t="s">
         <v>56</v>
@@ -2732,7 +2735,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="25" t="n">
         <v>69</v>
       </c>
@@ -2743,22 +2746,22 @@
         <v>49</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F23" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G23" s="28" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H23" s="28" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I23" s="28" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J23" s="29" t="s">
         <v>56</v>
@@ -2784,7 +2787,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="25" t="n">
         <v>70</v>
       </c>
@@ -2795,22 +2798,22 @@
         <v>49</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F24" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G24" s="28" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H24" s="28" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I24" s="28" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J24" s="29" t="s">
         <v>56</v>
@@ -2847,10 +2850,10 @@
         <v>49</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E25" s="27" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F25" s="28"/>
       <c r="G25" s="34"/>
@@ -2860,7 +2863,7 @@
         <v>76</v>
       </c>
       <c r="K25" s="29" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L25" s="29"/>
       <c r="M25" s="29"/>
@@ -2885,10 +2888,10 @@
         <v>49</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E26" s="27" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F26" s="28"/>
       <c r="G26" s="34"/>
@@ -2898,7 +2901,7 @@
         <v>76</v>
       </c>
       <c r="K26" s="29" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L26" s="29"/>
       <c r="M26" s="29"/>
@@ -2923,10 +2926,10 @@
         <v>49</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E27" s="27" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F27" s="28"/>
       <c r="G27" s="34"/>
@@ -2936,7 +2939,7 @@
         <v>76</v>
       </c>
       <c r="K27" s="29" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L27" s="29"/>
       <c r="M27" s="29"/>
@@ -2961,10 +2964,10 @@
         <v>49</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E28" s="27" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F28" s="28"/>
       <c r="G28" s="28"/>
@@ -2974,7 +2977,7 @@
         <v>76</v>
       </c>
       <c r="K28" s="29" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L28" s="29"/>
       <c r="M28" s="29"/>
@@ -2988,7 +2991,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="114.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="25" t="n">
         <v>32</v>
       </c>
@@ -2996,10 +2999,10 @@
         <v>48</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E29" s="33" t="s">
         <v>73</v>
@@ -3008,10 +3011,10 @@
         <v>52</v>
       </c>
       <c r="G29" s="28" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H29" s="28" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I29" s="28" t="s">
         <v>75</v>
@@ -3040,7 +3043,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="25" t="n">
         <v>40</v>
       </c>
@@ -3048,10 +3051,10 @@
         <v>48</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E30" s="33" t="s">
         <v>80</v>
@@ -3060,10 +3063,10 @@
         <v>52</v>
       </c>
       <c r="G30" s="28" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H30" s="28" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I30" s="28" t="s">
         <v>75</v>
@@ -3092,7 +3095,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="102.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="25" t="n">
         <v>48</v>
       </c>
@@ -3100,10 +3103,10 @@
         <v>48</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E31" s="27" t="s">
         <v>84</v>
@@ -3136,25 +3139,25 @@
         <v>48</v>
       </c>
       <c r="C32" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F32" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G32" s="28" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H32" s="28" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I32" s="28" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J32" s="29" t="s">
         <v>56</v>
@@ -3180,25 +3183,25 @@
         <v>48</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E33" s="27" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F33" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G33" s="28" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H33" s="28" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I33" s="28" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J33" s="29" t="s">
         <v>56</v>
@@ -3224,25 +3227,25 @@
         <v>48</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E34" s="27" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F34" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G34" s="28" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H34" s="28" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="I34" s="28" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="J34" s="29" t="s">
         <v>56</v>
@@ -3268,25 +3271,25 @@
         <v>48</v>
       </c>
       <c r="C35" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E35" s="27" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F35" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G35" s="28" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H35" s="28" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I35" s="28" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="J35" s="29" t="s">
         <v>56</v>
@@ -3304,7 +3307,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="25" t="n">
         <v>151</v>
       </c>
@@ -3312,25 +3315,25 @@
         <v>48</v>
       </c>
       <c r="C36" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E36" s="27" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F36" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G36" s="28" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H36" s="28" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I36" s="28" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="J36" s="29" t="s">
         <v>56</v>
@@ -3347,7 +3350,7 @@
         <v>56</v>
       </c>
       <c r="P36" s="29" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="Q36" s="29"/>
       <c r="R36" s="30"/>
@@ -3356,7 +3359,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="25" t="n">
         <v>152</v>
       </c>
@@ -3364,25 +3367,25 @@
         <v>48</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E37" s="27" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F37" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G37" s="28" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H37" s="28" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I37" s="28" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J37" s="29" t="s">
         <v>56</v>
@@ -3408,7 +3411,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="25" t="n">
         <v>153</v>
       </c>
@@ -3416,25 +3419,25 @@
         <v>48</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E38" s="27" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F38" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G38" s="28" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H38" s="28" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I38" s="28" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="J38" s="29" t="s">
         <v>56</v>
@@ -3451,7 +3454,7 @@
         <v>56</v>
       </c>
       <c r="P38" s="29" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="Q38" s="29"/>
       <c r="R38" s="30"/>
@@ -3460,7 +3463,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="25" t="n">
         <v>154</v>
       </c>
@@ -3468,25 +3471,25 @@
         <v>48</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E39" s="27" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F39" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G39" s="28" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H39" s="28" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="I39" s="28" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="J39" s="29" t="s">
         <v>56</v>
@@ -3512,7 +3515,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="25" t="n">
         <v>155</v>
       </c>
@@ -3520,25 +3523,25 @@
         <v>48</v>
       </c>
       <c r="C40" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D40" s="26" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E40" s="27" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F40" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G40" s="28" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H40" s="28" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I40" s="28" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J40" s="29" t="s">
         <v>56</v>
@@ -3564,7 +3567,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="25" t="n">
         <v>156</v>
       </c>
@@ -3572,25 +3575,25 @@
         <v>48</v>
       </c>
       <c r="C41" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E41" s="27" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F41" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G41" s="28" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H41" s="28" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="I41" s="28" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J41" s="29" t="s">
         <v>56</v>
@@ -3616,7 +3619,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="25" t="n">
         <v>157</v>
       </c>
@@ -3624,25 +3627,25 @@
         <v>48</v>
       </c>
       <c r="C42" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D42" s="26" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E42" s="27" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F42" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G42" s="28" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H42" s="28" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I42" s="28" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J42" s="29" t="s">
         <v>56</v>
@@ -3668,7 +3671,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="25" t="n">
         <v>158</v>
       </c>
@@ -3676,25 +3679,25 @@
         <v>48</v>
       </c>
       <c r="C43" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E43" s="27" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F43" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G43" s="28" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H43" s="28" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="I43" s="28" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="J43" s="29" t="s">
         <v>56</v>
@@ -3720,7 +3723,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="25" t="n">
         <v>159</v>
       </c>
@@ -3728,25 +3731,25 @@
         <v>48</v>
       </c>
       <c r="C44" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D44" s="26" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E44" s="27" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F44" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G44" s="28" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H44" s="28" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="I44" s="28" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="J44" s="29" t="s">
         <v>56</v>
@@ -3772,7 +3775,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="25" t="n">
         <v>160</v>
       </c>
@@ -3780,25 +3783,25 @@
         <v>48</v>
       </c>
       <c r="C45" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E45" s="27" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F45" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G45" s="28" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H45" s="28" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I45" s="28" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="J45" s="29" t="s">
         <v>56</v>
@@ -3824,7 +3827,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="25" t="n">
         <v>161</v>
       </c>
@@ -3832,25 +3835,25 @@
         <v>48</v>
       </c>
       <c r="C46" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E46" s="27" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F46" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G46" s="28" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H46" s="28" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="I46" s="28" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="J46" s="29" t="s">
         <v>56</v>
@@ -3876,7 +3879,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="25" t="n">
         <v>162</v>
       </c>
@@ -3884,25 +3887,25 @@
         <v>48</v>
       </c>
       <c r="C47" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D47" s="26" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E47" s="27" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F47" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G47" s="28" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H47" s="28" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="I47" s="28" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="J47" s="29" t="s">
         <v>56</v>
@@ -3936,13 +3939,13 @@
         <v>48</v>
       </c>
       <c r="C48" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E48" s="27" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F48" s="28"/>
       <c r="G48" s="34"/>
@@ -3952,7 +3955,7 @@
         <v>76</v>
       </c>
       <c r="K48" s="29" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L48" s="29"/>
       <c r="M48" s="29"/>
@@ -3974,13 +3977,13 @@
         <v>48</v>
       </c>
       <c r="C49" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D49" s="26" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E49" s="27" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F49" s="28"/>
       <c r="G49" s="34"/>
@@ -3990,7 +3993,7 @@
         <v>76</v>
       </c>
       <c r="K49" s="29" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L49" s="29"/>
       <c r="M49" s="29"/>
@@ -4012,13 +4015,13 @@
         <v>48</v>
       </c>
       <c r="C50" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D50" s="26" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E50" s="27" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F50" s="28"/>
       <c r="G50" s="34"/>
@@ -4028,7 +4031,7 @@
         <v>76</v>
       </c>
       <c r="K50" s="29" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L50" s="29"/>
       <c r="M50" s="29"/>
@@ -4050,13 +4053,13 @@
         <v>48</v>
       </c>
       <c r="C51" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D51" s="26" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E51" s="27" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F51" s="28"/>
       <c r="G51" s="34"/>
@@ -4066,7 +4069,7 @@
         <v>76</v>
       </c>
       <c r="K51" s="29" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L51" s="29"/>
       <c r="M51" s="29"/>
@@ -4088,13 +4091,13 @@
         <v>48</v>
       </c>
       <c r="C52" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D52" s="26" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E52" s="27" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F52" s="28"/>
       <c r="G52" s="34"/>
@@ -4104,7 +4107,7 @@
         <v>76</v>
       </c>
       <c r="K52" s="29" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L52" s="29"/>
       <c r="M52" s="29"/>
@@ -4118,7 +4121,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="25" t="n">
         <v>168</v>
       </c>
@@ -4126,25 +4129,25 @@
         <v>48</v>
       </c>
       <c r="C53" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D53" s="26" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E53" s="27" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="F53" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G53" s="28" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H53" s="28" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="I53" s="28" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="J53" s="29" t="s">
         <v>56</v>
@@ -4170,7 +4173,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="25" t="n">
         <v>169</v>
       </c>
@@ -4178,25 +4181,25 @@
         <v>48</v>
       </c>
       <c r="C54" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D54" s="26" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E54" s="27" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F54" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G54" s="28" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H54" s="28" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I54" s="28" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="J54" s="29" t="s">
         <v>56</v>
@@ -10619,24 +10622,24 @@
         <v>29</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10644,125 +10647,125 @@
         <v>49</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C10" s="35" t="n">
         <v>191</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C11" s="35" t="n">
         <v>192</v>
       </c>
       <c r="D11" s="35" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10770,111 +10773,111 @@
         <v>49</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C12" s="35" t="n">
         <v>208</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C13" s="35" t="n">
         <v>224</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C14" s="35" t="n">
         <v>240</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C15" s="35" t="n">
         <v>256</v>
       </c>
       <c r="D15" s="36" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C16" s="35" t="n">
         <v>272</v>
       </c>
       <c r="D16" s="36" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C17" s="35" t="n">
         <v>288</v>
       </c>
       <c r="D17" s="36" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C18" s="35" t="n">
         <v>304</v>
       </c>
       <c r="D18" s="36" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C19" s="35" t="n">
         <v>193</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10882,111 +10885,111 @@
         <v>49</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C20" s="35" t="n">
         <v>209</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C21" s="35" t="n">
         <v>225</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C22" s="35" t="n">
         <v>241</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C23" s="35" t="n">
         <v>257</v>
       </c>
       <c r="D23" s="36" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C24" s="35" t="n">
         <v>273</v>
       </c>
       <c r="D24" s="36" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C25" s="35" t="n">
         <v>289</v>
       </c>
       <c r="D25" s="36" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="11" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C26" s="35" t="n">
         <v>305</v>
       </c>
       <c r="D26" s="36" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="11" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C27" s="35" t="n">
         <v>194</v>
       </c>
       <c r="D27" s="35" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10994,105 +10997,105 @@
         <v>49</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C28" s="35" t="n">
         <v>210</v>
       </c>
       <c r="D28" s="35" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C29" s="35" t="n">
         <v>226</v>
       </c>
       <c r="D29" s="37" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="11" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C30" s="35" t="n">
         <v>242</v>
       </c>
       <c r="D30" s="35" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C31" s="35" t="n">
         <v>258</v>
       </c>
       <c r="D31" s="36" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C32" s="35" t="n">
         <v>274</v>
       </c>
       <c r="D32" s="36" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C33" s="35" t="n">
         <v>290</v>
       </c>
       <c r="D33" s="36" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="11" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C34" s="35" t="n">
         <v>306</v>
       </c>
       <c r="D34" s="36" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="11" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C35" s="35" t="n">
         <v>195</v>
@@ -11106,7 +11109,7 @@
         <v>49</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C36" s="35" t="n">
         <v>211</v>
@@ -11117,10 +11120,10 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="11" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C37" s="35" t="n">
         <v>227</v>
@@ -11131,10 +11134,10 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="11" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C38" s="35" t="n">
         <v>243</v>
@@ -11145,10 +11148,10 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="11" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C39" s="35" t="n">
         <v>259</v>
@@ -11159,10 +11162,10 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C40" s="35" t="n">
         <v>275</v>
@@ -11173,10 +11176,10 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C41" s="35" t="n">
         <v>291</v>
@@ -11187,10 +11190,10 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="11" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C42" s="35" t="n">
         <v>307</v>
@@ -11201,10 +11204,10 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="11" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C43" s="35" t="n">
         <v>196</v>
@@ -11218,7 +11221,7 @@
         <v>49</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C44" s="35" t="n">
         <v>212</v>
@@ -11229,10 +11232,10 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="11" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C45" s="35" t="n">
         <v>228</v>
@@ -11243,10 +11246,10 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="11" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C46" s="35" t="n">
         <v>244</v>
@@ -11257,10 +11260,10 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="11" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C47" s="35" t="n">
         <v>260</v>
@@ -11271,10 +11274,10 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C48" s="35" t="n">
         <v>276</v>
@@ -11285,10 +11288,10 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C49" s="35" t="n">
         <v>292</v>
@@ -11299,10 +11302,10 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="11" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C50" s="35" t="n">
         <v>308</v>
@@ -11350,7 +11353,7 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="38" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B2" s="38" t="s">
         <v>56</v>
@@ -11358,7 +11361,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="38" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B3" s="38" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
Aggiornamento colonna GESTIONE ERRORE nel file report-checklist.xlsx
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#090903000000XX/AOUCAREGGI/ARCHIMED/8.48/report-checklist.xlsx
+++ b/GATEWAY/A1#090903000000XX/AOUCAREGGI/ARCHIMED/8.48/report-checklist.xlsx
@@ -422,7 +422,7 @@
     <t xml:space="preserve">NO</t>
   </si>
   <si>
-    <t xml:space="preserve">L'invio al gateway è asincrono e il medico prosegue con la propria attività. In caso di errore viene inviata al medico e al personale amministrativo una notifica. Dopo che l'errore è stato corretto dal medico o dal personale amministrativo, il referto può essere firmato nuovamente e inviato alla coda che in maniera automatica e schedulata (intervallo configurabile) ritenta l’invio verso il gateway </t>
+    <t xml:space="preserve">L'invio al gateway è asincrono per permettere al medico di proseguire con la propria attività clinica. Sia il medico che il backoffice hanno a disposizione un cruscotto che mostra i messaggi non andati a buon fine con la descrizione dell'errore. Una volta che l'errore è stato corretto dal medico o dal backoffice, il documento rientra nella coda di firma e di ritrasmissione verso il gateway.</t>
   </si>
   <si>
     <t xml:space="preserve">KO</t>
@@ -511,7 +511,7 @@
     <t xml:space="preserve">2.16.840.1.113883.2.9.2.90903.45c9c160458635a842a60b21f2db53b82a1a6d5d071ffca01fa8fc826915cbf3.2fc5e5addb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t xml:space="preserve">L'invio al gateway è asincrono e il medico prosegue con la propria attività. In caso di errore viene inviata al medico e al personale amministrativo una notifica. Dopo che l'errore è stato corretto dal medico, il referto può essere firmato nuovamente e inviato alla coda che in maniera automatica e schedulata (intervallo configurabile) ritenta l’invio verso il gateway </t>
+    <t xml:space="preserve">L'invio al gateway è asincrono per permettere al medico di proseguire con la propria attività clinica. Sia il medico che il backoffice hanno a disposizione un cruscotto che mostra i messaggi non andati a buon fine con la descrizione dell'errore. Una volta che l'errore è stato corretto dal medico, in maniera autonoma o su segnalazione del backoffice, il documento rientra nella coda di firma e di ritrasmissione verso il gateway.</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT6_KO</t>
@@ -1867,11 +1867,11 @@
   <dimension ref="A1:T581"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="J25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="J7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
-      <selection pane="bottomRight" activeCell="P53" activeCellId="0" sqref="P53"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="P36" activeCellId="0" sqref="P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2285,7 +2285,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="25" t="n">
         <v>29</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="25" t="n">
         <v>37</v>
       </c>
@@ -2423,7 +2423,7 @@
       <c r="S16" s="31"/>
       <c r="T16" s="32"/>
     </row>
-    <row r="17" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="25" t="n">
         <v>63</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="25" t="n">
         <v>64</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="170.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="25" t="n">
         <v>65</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="25" t="n">
         <v>66</v>
       </c>
@@ -2631,7 +2631,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="25" t="n">
         <v>67</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="25" t="n">
         <v>68</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="25" t="n">
         <v>69</v>
       </c>
@@ -2787,7 +2787,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="25" t="n">
         <v>70</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="25" t="n">
         <v>32</v>
       </c>
@@ -3043,7 +3043,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="25" t="n">
         <v>40</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="170.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="25" t="n">
         <v>151</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="25" t="n">
         <v>152</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="170.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="25" t="n">
         <v>153</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="25" t="n">
         <v>154</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="25" t="n">
         <v>155</v>
       </c>
@@ -3567,7 +3567,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="25" t="n">
         <v>156</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="25" t="n">
         <v>157</v>
       </c>
@@ -3671,7 +3671,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="25" t="n">
         <v>158</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="25" t="n">
         <v>159</v>
       </c>
@@ -3775,7 +3775,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="25" t="n">
         <v>160</v>
       </c>
@@ -3827,7 +3827,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="25" t="n">
         <v>161</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="25" t="n">
         <v>162</v>
       </c>
@@ -4121,7 +4121,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="25" t="n">
         <v>168</v>
       </c>
@@ -4173,7 +4173,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="25" t="n">
         <v>169</v>
       </c>

</xml_diff>